<commit_message>
added figures and tables
</commit_message>
<xml_diff>
--- a/quanti_vals.xlsx
+++ b/quanti_vals.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,11 @@
           <t>lb</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -553,6 +558,9 @@
       <c r="O2" t="n">
         <v>1</v>
       </c>
+      <c r="P2" t="n">
+        <v>513</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -602,6 +610,9 @@
       <c r="O3" t="n">
         <v>14</v>
       </c>
+      <c r="P3" t="n">
+        <v>763</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -651,6 +662,9 @@
       <c r="O4" t="n">
         <v>3</v>
       </c>
+      <c r="P4" t="n">
+        <v>676</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -700,6 +714,9 @@
       <c r="O5" t="n">
         <v>1</v>
       </c>
+      <c r="P5" t="n">
+        <v>307</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -749,6 +766,9 @@
       <c r="O6" t="n">
         <v>1</v>
       </c>
+      <c r="P6" t="n">
+        <v>320</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -797,6 +817,9 @@
       </c>
       <c r="O7" t="n">
         <v>1</v>
+      </c>
+      <c r="P7" t="n">
+        <v>282</v>
       </c>
     </row>
     <row r="8">
@@ -847,6 +870,9 @@
       <c r="O8" t="n">
         <v>11</v>
       </c>
+      <c r="P8" t="n">
+        <v>592</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -896,6 +922,9 @@
       <c r="O9" t="n">
         <v>10</v>
       </c>
+      <c r="P9" t="n">
+        <v>873</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -945,6 +974,9 @@
       <c r="O10" t="n">
         <v>0</v>
       </c>
+      <c r="P10" t="n">
+        <v>325</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -994,6 +1026,9 @@
       <c r="O11" t="n">
         <v>2</v>
       </c>
+      <c r="P11" t="n">
+        <v>343</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1043,6 +1078,9 @@
       <c r="O12" t="n">
         <v>2</v>
       </c>
+      <c r="P12" t="n">
+        <v>772</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1092,6 +1130,9 @@
       <c r="O13" t="n">
         <v>23</v>
       </c>
+      <c r="P13" t="n">
+        <v>720</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1141,6 +1182,9 @@
       <c r="O14" t="n">
         <v>0</v>
       </c>
+      <c r="P14" t="n">
+        <v>358</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1190,6 +1234,9 @@
       <c r="O15" t="n">
         <v>1</v>
       </c>
+      <c r="P15" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1239,6 +1286,9 @@
       <c r="O16" t="n">
         <v>35</v>
       </c>
+      <c r="P16" t="n">
+        <v>794</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1288,6 +1338,9 @@
       <c r="O17" t="n">
         <v>20</v>
       </c>
+      <c r="P17" t="n">
+        <v>644</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1337,6 +1390,9 @@
       <c r="O18" t="n">
         <v>1</v>
       </c>
+      <c r="P18" t="n">
+        <v>372</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1386,6 +1442,9 @@
       <c r="O19" t="n">
         <v>29</v>
       </c>
+      <c r="P19" t="n">
+        <v>1020</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1435,6 +1494,9 @@
       <c r="O20" t="n">
         <v>15</v>
       </c>
+      <c r="P20" t="n">
+        <v>358</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1484,6 +1546,9 @@
       <c r="O21" t="n">
         <v>40</v>
       </c>
+      <c r="P21" t="n">
+        <v>900</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1533,6 +1598,9 @@
       <c r="O22" t="n">
         <v>41</v>
       </c>
+      <c r="P22" t="n">
+        <v>1126</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1582,6 +1650,9 @@
       <c r="O23" t="n">
         <v>4</v>
       </c>
+      <c r="P23" t="n">
+        <v>320</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1631,6 +1702,9 @@
       <c r="O24" t="n">
         <v>3</v>
       </c>
+      <c r="P24" t="n">
+        <v>338</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1680,6 +1754,9 @@
       <c r="O25" t="n">
         <v>6</v>
       </c>
+      <c r="P25" t="n">
+        <v>407</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1729,6 +1806,9 @@
       <c r="O26" t="n">
         <v>14</v>
       </c>
+      <c r="P26" t="n">
+        <v>651</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1778,6 +1858,9 @@
       <c r="O27" t="n">
         <v>4</v>
       </c>
+      <c r="P27" t="n">
+        <v>1099</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1827,6 +1910,9 @@
       <c r="O28" t="n">
         <v>8</v>
       </c>
+      <c r="P28" t="n">
+        <v>415</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1876,6 +1962,9 @@
       <c r="O29" t="n">
         <v>6</v>
       </c>
+      <c r="P29" t="n">
+        <v>475</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1925,6 +2014,9 @@
       <c r="O30" t="n">
         <v>3</v>
       </c>
+      <c r="P30" t="n">
+        <v>475</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1974,6 +2066,9 @@
       <c r="O31" t="n">
         <v>40</v>
       </c>
+      <c r="P31" t="n">
+        <v>1018</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2023,6 +2118,9 @@
       <c r="O32" t="n">
         <v>12</v>
       </c>
+      <c r="P32" t="n">
+        <v>786</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2072,6 +2170,9 @@
       <c r="O33" t="n">
         <v>21</v>
       </c>
+      <c r="P33" t="n">
+        <v>1161</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2121,6 +2222,9 @@
       <c r="O34" t="n">
         <v>16</v>
       </c>
+      <c r="P34" t="n">
+        <v>839</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2170,6 +2274,9 @@
       <c r="O35" t="n">
         <v>2</v>
       </c>
+      <c r="P35" t="n">
+        <v>458</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2219,6 +2326,9 @@
       <c r="O36" t="n">
         <v>7</v>
       </c>
+      <c r="P36" t="n">
+        <v>915</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2268,6 +2378,9 @@
       <c r="O37" t="n">
         <v>12</v>
       </c>
+      <c r="P37" t="n">
+        <v>786</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2317,6 +2430,9 @@
       <c r="O38" t="n">
         <v>2</v>
       </c>
+      <c r="P38" t="n">
+        <v>760</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2366,6 +2482,9 @@
       <c r="O39" t="n">
         <v>22</v>
       </c>
+      <c r="P39" t="n">
+        <v>459</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2415,6 +2534,9 @@
       <c r="O40" t="n">
         <v>7</v>
       </c>
+      <c r="P40" t="n">
+        <v>856</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2464,6 +2586,9 @@
       <c r="O41" t="n">
         <v>2</v>
       </c>
+      <c r="P41" t="n">
+        <v>437</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2513,6 +2638,9 @@
       <c r="O42" t="n">
         <v>14</v>
       </c>
+      <c r="P42" t="n">
+        <v>804</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2562,6 +2690,9 @@
       <c r="O43" t="n">
         <v>18</v>
       </c>
+      <c r="P43" t="n">
+        <v>530</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2611,6 +2742,9 @@
       <c r="O44" t="n">
         <v>2</v>
       </c>
+      <c r="P44" t="n">
+        <v>931</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2660,6 +2794,9 @@
       <c r="O45" t="n">
         <v>4</v>
       </c>
+      <c r="P45" t="n">
+        <v>414</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2709,6 +2846,9 @@
       <c r="O46" t="n">
         <v>12</v>
       </c>
+      <c r="P46" t="n">
+        <v>736</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2758,6 +2898,9 @@
       <c r="O47" t="n">
         <v>6</v>
       </c>
+      <c r="P47" t="n">
+        <v>408</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2807,6 +2950,9 @@
       <c r="O48" t="n">
         <v>4</v>
       </c>
+      <c r="P48" t="n">
+        <v>697</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2856,6 +3002,9 @@
       <c r="O49" t="n">
         <v>1</v>
       </c>
+      <c r="P49" t="n">
+        <v>277</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2905,6 +3054,9 @@
       <c r="O50" t="n">
         <v>11</v>
       </c>
+      <c r="P50" t="n">
+        <v>1134</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2954,6 +3106,9 @@
       <c r="O51" t="n">
         <v>23</v>
       </c>
+      <c r="P51" t="n">
+        <v>762</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -3003,6 +3158,9 @@
       <c r="O52" t="n">
         <v>7</v>
       </c>
+      <c r="P52" t="n">
+        <v>697</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -3052,6 +3210,9 @@
       <c r="O53" t="n">
         <v>17</v>
       </c>
+      <c r="P53" t="n">
+        <v>489</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -3101,6 +3262,9 @@
       <c r="O54" t="n">
         <v>3</v>
       </c>
+      <c r="P54" t="n">
+        <v>415</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -3150,6 +3314,9 @@
       <c r="O55" t="n">
         <v>2</v>
       </c>
+      <c r="P55" t="n">
+        <v>224</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -3199,6 +3366,9 @@
       <c r="O56" t="n">
         <v>11</v>
       </c>
+      <c r="P56" t="n">
+        <v>746</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -3248,6 +3418,9 @@
       <c r="O57" t="n">
         <v>11</v>
       </c>
+      <c r="P57" t="n">
+        <v>577</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -3297,6 +3470,9 @@
       <c r="O58" t="n">
         <v>3</v>
       </c>
+      <c r="P58" t="n">
+        <v>455</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -3346,6 +3522,9 @@
       <c r="O59" t="n">
         <v>10</v>
       </c>
+      <c r="P59" t="n">
+        <v>550</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -3395,6 +3574,9 @@
       <c r="O60" t="n">
         <v>15</v>
       </c>
+      <c r="P60" t="n">
+        <v>486</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -3443,6 +3625,9 @@
       </c>
       <c r="O61" t="n">
         <v>1</v>
+      </c>
+      <c r="P61" t="n">
+        <v>319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>